<commit_message>
mods to dreadin macro: 30yr apr, bonds, bills added
</commit_message>
<xml_diff>
--- a/readin/dsreadin_macro_data.xlsx
+++ b/readin/dsreadin_macro_data.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="15">
   <si>
     <t>YEAR</t>
   </si>
@@ -61,6 +61,15 @@
   </si>
   <si>
     <t>inf_act</t>
+  </si>
+  <si>
+    <t>apr30yr</t>
+  </si>
+  <si>
+    <t>tbill1yr</t>
+  </si>
+  <si>
+    <t>tbond10yr</t>
   </si>
 </sst>
 </file>
@@ -107,7 +116,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -119,6 +128,7 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -399,10 +409,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H114"/>
+  <dimension ref="A1:K114"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+      <selection activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -411,9 +421,10 @@
     <col min="4" max="5" width="12.140625" customWidth="1"/>
     <col min="6" max="6" width="10.85546875" customWidth="1"/>
     <col min="7" max="7" width="8.28515625" customWidth="1"/>
+    <col min="11" max="11" width="10" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -438,8 +449,17 @@
       <c r="H1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I1" t="s">
+        <v>13</v>
+      </c>
+      <c r="J1" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="K1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1986</v>
       </c>
@@ -464,8 +484,17 @@
       <c r="H2">
         <v>2.1535600000000002E-2</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I2">
+        <v>7.0300000000000001E-2</v>
+      </c>
+      <c r="J2">
+        <v>0.10099999999999999</v>
+      </c>
+      <c r="K2">
+        <v>7.7800000000000008E-2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1986</v>
       </c>
@@ -490,8 +519,17 @@
       <c r="H3">
         <v>1.76744E-2</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I3">
+        <v>6.7300000000000013E-2</v>
+      </c>
+      <c r="J3">
+        <v>0.10619999999999999</v>
+      </c>
+      <c r="K3">
+        <v>7.8E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>1986</v>
       </c>
@@ -516,8 +554,17 @@
       <c r="H4">
         <v>1.75763E-2</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I4">
+        <v>5.7699999999999994E-2</v>
+      </c>
+      <c r="J4">
+        <v>0.10099999999999999</v>
+      </c>
+      <c r="K4">
+        <v>7.4499999999999997E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>1986</v>
       </c>
@@ -542,8 +589,17 @@
       <c r="H5">
         <v>1.1872100000000002E-2</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I5">
+        <v>5.8700000000000002E-2</v>
+      </c>
+      <c r="J5">
+        <v>9.2899999999999996E-2</v>
+      </c>
+      <c r="K5">
+        <v>7.110000000000001E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>1987</v>
       </c>
@@ -568,8 +624,17 @@
       <c r="H6">
         <v>2.84143E-2</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I6">
+        <v>6.0300000000000006E-2</v>
+      </c>
+      <c r="J6">
+        <v>9.0299999999999991E-2</v>
+      </c>
+      <c r="K6">
+        <v>7.2499999999999995E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>1987</v>
       </c>
@@ -594,8 +659,17 @@
       <c r="H7">
         <v>3.7477099999999999E-2</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I7">
+        <v>6.8000000000000005E-2</v>
+      </c>
+      <c r="J7">
+        <v>0.10349999999999999</v>
+      </c>
+      <c r="K7">
+        <v>8.4000000000000005E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>1987</v>
       </c>
@@ -620,8 +694,17 @@
       <c r="H8">
         <v>4.2727300000000003E-2</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I8">
+        <v>7.6700000000000004E-2</v>
+      </c>
+      <c r="J8">
+        <v>0.11019999999999999</v>
+      </c>
+      <c r="K8">
+        <v>9.4200000000000006E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>1987</v>
       </c>
@@ -646,8 +729,17 @@
       <c r="H9">
         <v>4.33213E-2</v>
       </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I9">
+        <v>7.17E-2</v>
+      </c>
+      <c r="J9">
+        <v>0.1061</v>
+      </c>
+      <c r="K9">
+        <v>8.9900000000000008E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>1988</v>
       </c>
@@ -672,8 +764,17 @@
       <c r="H10">
         <v>3.8324400000000002E-2</v>
       </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I10">
+        <v>6.7100000000000007E-2</v>
+      </c>
+      <c r="J10">
+        <v>9.9900000000000003E-2</v>
+      </c>
+      <c r="K10">
+        <v>8.3699999999999997E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>1988</v>
       </c>
@@ -698,8 +799,17 @@
       <c r="H11">
         <v>3.9647599999999998E-2</v>
       </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I11">
+        <v>7.4900000000000008E-2</v>
+      </c>
+      <c r="J11">
+        <v>0.10400000000000001</v>
+      </c>
+      <c r="K11">
+        <v>8.9200000000000002E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>1988</v>
       </c>
@@ -724,8 +834,17 @@
       <c r="H12">
         <v>4.1848299999999998E-2</v>
       </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I12">
+        <v>8.09E-2</v>
+      </c>
+      <c r="J12">
+        <v>0.1042</v>
+      </c>
+      <c r="K12">
+        <v>8.9800000000000005E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>1988</v>
       </c>
@@ -750,8 +869,17 @@
       <c r="H13">
         <v>4.41176E-2</v>
       </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I13">
+        <v>8.9900000000000008E-2</v>
+      </c>
+      <c r="J13">
+        <v>0.1077</v>
+      </c>
+      <c r="K13">
+        <v>9.11E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>1989</v>
       </c>
@@ -776,8 +904,17 @@
       <c r="H14">
         <v>4.8926999999999998E-2</v>
       </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I14">
+        <v>9.5700000000000007E-2</v>
+      </c>
+      <c r="J14">
+        <v>0.1119</v>
+      </c>
+      <c r="K14">
+        <v>9.3600000000000003E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>1989</v>
       </c>
@@ -802,8 +939,17 @@
       <c r="H15">
         <v>5.1694899999999995E-2</v>
       </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I15">
+        <v>8.4400000000000003E-2</v>
+      </c>
+      <c r="J15">
+        <v>0.10070000000000001</v>
+      </c>
+      <c r="K15">
+        <v>8.2799999999999999E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>1989</v>
       </c>
@@ -828,8 +974,17 @@
       <c r="H16">
         <v>4.4351500000000002E-2</v>
       </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I16">
+        <v>8.2200000000000009E-2</v>
+      </c>
+      <c r="J16">
+        <v>0.10160000000000001</v>
+      </c>
+      <c r="K16">
+        <v>8.1900000000000001E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>1989</v>
       </c>
@@ -854,8 +1009,17 @@
       <c r="H17">
         <v>4.6396E-2</v>
       </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I17">
+        <v>7.7200000000000005E-2</v>
+      </c>
+      <c r="J17">
+        <v>9.7799999999999998E-2</v>
+      </c>
+      <c r="K17">
+        <v>7.8399999999999997E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>1990</v>
       </c>
@@ -880,8 +1044,17 @@
       <c r="H18">
         <v>5.2373200000000009E-2</v>
       </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I18">
+        <v>8.3500000000000005E-2</v>
+      </c>
+      <c r="J18">
+        <v>0.10220000000000001</v>
+      </c>
+      <c r="K18">
+        <v>8.5900000000000004E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>1990</v>
       </c>
@@ -906,8 +1079,17 @@
       <c r="H19">
         <v>4.6736500000000007E-2</v>
       </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I19">
+        <v>8.1000000000000003E-2</v>
+      </c>
+      <c r="J19">
+        <v>0.10150000000000001</v>
+      </c>
+      <c r="K19">
+        <v>8.48E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>1990</v>
       </c>
@@ -932,8 +1114,17 @@
       <c r="H20">
         <v>6.1698700000000002E-2</v>
       </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I20">
+        <v>7.7600000000000002E-2</v>
+      </c>
+      <c r="J20">
+        <v>0.10220000000000001</v>
+      </c>
+      <c r="K20">
+        <v>8.8900000000000007E-2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>1990</v>
       </c>
@@ -958,8 +1149,17 @@
       <c r="H21">
         <v>6.2549500000000008E-2</v>
       </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I21">
+        <v>7.0499999999999993E-2</v>
+      </c>
+      <c r="J21">
+        <v>9.6799999999999997E-2</v>
+      </c>
+      <c r="K21">
+        <v>8.0799999999999997E-2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>1991</v>
       </c>
@@ -984,8 +1184,17 @@
       <c r="H22">
         <v>4.8211500000000004E-2</v>
       </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I22">
+        <v>6.4000000000000001E-2</v>
+      </c>
+      <c r="J22">
+        <v>9.5199999999999993E-2</v>
+      </c>
+      <c r="K22">
+        <v>8.1099999999999992E-2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>1991</v>
       </c>
@@ -1010,8 +1219,17 @@
       <c r="H23">
         <v>4.69592E-2</v>
       </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I23">
+        <v>6.3600000000000004E-2</v>
+      </c>
+      <c r="J23">
+        <v>9.6700000000000008E-2</v>
+      </c>
+      <c r="K23">
+        <v>8.2799999999999999E-2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>1991</v>
       </c>
@@ -1036,8 +1254,17 @@
       <c r="H24">
         <v>3.3962300000000001E-2</v>
       </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I24">
+        <v>5.5700000000000006E-2</v>
+      </c>
+      <c r="J24">
+        <v>8.9200000000000002E-2</v>
+      </c>
+      <c r="K24">
+        <v>7.6499999999999999E-2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>1991</v>
       </c>
@@ -1062,8 +1289,17 @@
       <c r="H25">
         <v>2.9806300000000001E-2</v>
       </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I25">
+        <v>4.3799999999999999E-2</v>
+      </c>
+      <c r="J25">
+        <v>8.3500000000000005E-2</v>
+      </c>
+      <c r="K25">
+        <v>7.0900000000000005E-2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>1992</v>
       </c>
@@ -1088,8 +1324,17 @@
       <c r="H26">
         <v>3.18991E-2</v>
       </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I26">
+        <v>4.6300000000000001E-2</v>
+      </c>
+      <c r="J26">
+        <v>8.9800000000000005E-2</v>
+      </c>
+      <c r="K26">
+        <v>7.5400000000000009E-2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>1992</v>
       </c>
@@ -1114,8 +1359,17 @@
       <c r="H27">
         <v>3.01471E-2</v>
       </c>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I27">
+        <v>4.1700000000000001E-2</v>
+      </c>
+      <c r="J27">
+        <v>8.43E-2</v>
+      </c>
+      <c r="K27">
+        <v>7.2599999999999998E-2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>1992</v>
       </c>
@@ -1140,8 +1394,17 @@
       <c r="H28">
         <v>2.9927000000000002E-2</v>
       </c>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I28">
+        <v>3.1800000000000002E-2</v>
+      </c>
+      <c r="J28">
+        <v>8.0199999999999994E-2</v>
+      </c>
+      <c r="K28">
+        <v>6.4200000000000007E-2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>1992</v>
       </c>
@@ -1166,8 +1429,17 @@
       <c r="H29">
         <v>2.9667100000000002E-2</v>
       </c>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I29">
+        <v>3.7100000000000001E-2</v>
+      </c>
+      <c r="J29">
+        <v>8.1400000000000014E-2</v>
+      </c>
+      <c r="K29">
+        <v>6.7699999999999996E-2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>1993</v>
       </c>
@@ -1192,8 +1464,17 @@
       <c r="H30">
         <v>3.0194100000000001E-2</v>
       </c>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I30">
+        <v>3.3300000000000003E-2</v>
+      </c>
+      <c r="J30">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="K30">
+        <v>5.9800000000000006E-2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>1993</v>
       </c>
@@ -1218,8 +1499,17 @@
       <c r="H31">
         <v>2.9978600000000001E-2</v>
       </c>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I31">
+        <v>3.5400000000000001E-2</v>
+      </c>
+      <c r="J31">
+        <v>7.3400000000000007E-2</v>
+      </c>
+      <c r="K31">
+        <v>5.96E-2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>1993</v>
       </c>
@@ -1244,8 +1534,17 @@
       <c r="H32">
         <v>2.7639999999999998E-2</v>
       </c>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I32">
+        <v>3.3599999999999998E-2</v>
+      </c>
+      <c r="J32">
+        <v>6.9500000000000006E-2</v>
+      </c>
+      <c r="K32">
+        <v>5.3600000000000002E-2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>1993</v>
       </c>
@@ -1270,8 +1569,17 @@
       <c r="H33">
         <v>2.8109600000000002E-2</v>
       </c>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I33">
+        <v>3.61E-2</v>
+      </c>
+      <c r="J33">
+        <v>7.1300000000000002E-2</v>
+      </c>
+      <c r="K33">
+        <v>5.7699999999999994E-2</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>1994</v>
       </c>
@@ -1296,8 +1604,17 @@
       <c r="H34">
         <v>2.6517800000000001E-2</v>
       </c>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I34">
+        <v>4.3200000000000002E-2</v>
+      </c>
+      <c r="J34">
+        <v>7.8E-2</v>
+      </c>
+      <c r="K34">
+        <v>6.480000000000001E-2</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>1994</v>
       </c>
@@ -1322,8 +1639,17 @@
       <c r="H35">
         <v>2.4948000000000001E-2</v>
       </c>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I35">
+        <v>5.2699999999999997E-2</v>
+      </c>
+      <c r="J35">
+        <v>8.4600000000000009E-2</v>
+      </c>
+      <c r="K35">
+        <v>7.0999999999999994E-2</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>1994</v>
       </c>
@@ -1348,8 +1674,17 @@
       <c r="H36">
         <v>2.9655200000000003E-2</v>
       </c>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I36">
+        <v>5.7599999999999998E-2</v>
+      </c>
+      <c r="J36">
+        <v>8.8200000000000001E-2</v>
+      </c>
+      <c r="K36">
+        <v>7.46E-2</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>1994</v>
       </c>
@@ -1374,8 +1709,17 @@
       <c r="H37">
         <v>2.5974000000000001E-2</v>
       </c>
-    </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I37">
+        <v>7.1400000000000005E-2</v>
+      </c>
+      <c r="J37">
+        <v>9.1799999999999993E-2</v>
+      </c>
+      <c r="K37">
+        <v>7.8100000000000003E-2</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>1995</v>
       </c>
@@ -1400,8 +1744,17 @@
       <c r="H38">
         <v>2.78722E-2</v>
       </c>
-    </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I38">
+        <v>6.4299999999999996E-2</v>
+      </c>
+      <c r="J38">
+        <v>8.3800000000000013E-2</v>
+      </c>
+      <c r="K38">
+        <v>7.2000000000000008E-2</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>1995</v>
       </c>
@@ -1426,8 +1779,17 @@
       <c r="H39">
         <v>3.0426000000000002E-2</v>
       </c>
-    </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I39">
+        <v>5.6399999999999999E-2</v>
+      </c>
+      <c r="J39">
+        <v>7.5300000000000006E-2</v>
+      </c>
+      <c r="K39">
+        <v>6.1699999999999998E-2</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>1995</v>
       </c>
@@ -1452,8 +1814,17 @@
       <c r="H40">
         <v>2.5452100000000002E-2</v>
       </c>
-    </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I40">
+        <v>5.62E-2</v>
+      </c>
+      <c r="J40">
+        <v>7.6200000000000004E-2</v>
+      </c>
+      <c r="K40">
+        <v>6.2000000000000006E-2</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>1995</v>
       </c>
@@ -1478,8 +1849,17 @@
       <c r="H41">
         <v>2.5316499999999999E-2</v>
       </c>
-    </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I41">
+        <v>5.3099999999999994E-2</v>
+      </c>
+      <c r="J41">
+        <v>7.110000000000001E-2</v>
+      </c>
+      <c r="K41">
+        <v>5.7099999999999998E-2</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>1996</v>
       </c>
@@ -1504,8 +1884,17 @@
       <c r="H42">
         <v>2.8439199999999998E-2</v>
       </c>
-    </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I42">
+        <v>5.3400000000000003E-2</v>
+      </c>
+      <c r="J42">
+        <v>7.690000000000001E-2</v>
+      </c>
+      <c r="K42">
+        <v>6.2699999999999992E-2</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>1996</v>
       </c>
@@ -1530,8 +1919,17 @@
       <c r="H43">
         <v>2.8215199999999999E-2</v>
       </c>
-    </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I43">
+        <v>5.8099999999999999E-2</v>
+      </c>
+      <c r="J43">
+        <v>8.2899999999999988E-2</v>
+      </c>
+      <c r="K43">
+        <v>6.9100000000000009E-2</v>
+      </c>
+    </row>
+    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>1996</v>
       </c>
@@ -1556,8 +1954,17 @@
       <c r="H44">
         <v>3.0045700000000002E-2</v>
       </c>
-    </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I44">
+        <v>5.8300000000000005E-2</v>
+      </c>
+      <c r="J44">
+        <v>8.1600000000000006E-2</v>
+      </c>
+      <c r="K44">
+        <v>6.83E-2</v>
+      </c>
+    </row>
+    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>1996</v>
       </c>
@@ -1582,8 +1989,17 @@
       <c r="H45">
         <v>3.3788200000000004E-2</v>
       </c>
-    </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I45">
+        <v>5.4699999999999999E-2</v>
+      </c>
+      <c r="J45">
+        <v>7.6399999999999996E-2</v>
+      </c>
+      <c r="K45">
+        <v>6.3E-2</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>1997</v>
       </c>
@@ -1608,8 +2024,17 @@
       <c r="H46">
         <v>2.7652700000000002E-2</v>
       </c>
-    </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I46">
+        <v>5.7999999999999996E-2</v>
+      </c>
+      <c r="J46">
+        <v>7.9699999999999993E-2</v>
+      </c>
+      <c r="K46">
+        <v>6.6900000000000001E-2</v>
+      </c>
+    </row>
+    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>1997</v>
       </c>
@@ -1634,8 +2059,17 @@
       <c r="H47">
         <v>2.23357E-2</v>
       </c>
-    </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I47">
+        <v>5.6900000000000006E-2</v>
+      </c>
+      <c r="J47">
+        <v>7.5800000000000006E-2</v>
+      </c>
+      <c r="K47">
+        <v>6.4899999999999999E-2</v>
+      </c>
+    </row>
+    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>1997</v>
       </c>
@@ -1660,8 +2094,17 @@
       <c r="H48">
         <v>2.2193999999999998E-2</v>
       </c>
-    </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I48">
+        <v>5.5199999999999999E-2</v>
+      </c>
+      <c r="J48">
+        <v>7.2800000000000004E-2</v>
+      </c>
+      <c r="K48">
+        <v>6.2100000000000002E-2</v>
+      </c>
+    </row>
+    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>1997</v>
       </c>
@@ -1686,8 +2129,17 @@
       <c r="H49">
         <v>1.6970499999999999E-2</v>
       </c>
-    </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I49">
+        <v>5.5300000000000002E-2</v>
+      </c>
+      <c r="J49">
+        <v>6.9900000000000004E-2</v>
+      </c>
+      <c r="K49">
+        <v>5.8099999999999999E-2</v>
+      </c>
+    </row>
+    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>1998</v>
       </c>
@@ -1712,8 +2164,17 @@
       <c r="H50">
         <v>1.37672E-2</v>
       </c>
-    </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I50">
+        <v>5.3899999999999997E-2</v>
+      </c>
+      <c r="J50">
+        <v>7.0800000000000002E-2</v>
+      </c>
+      <c r="K50">
+        <v>5.6500000000000002E-2</v>
+      </c>
+    </row>
+    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>1998</v>
       </c>
@@ -1738,8 +2199,17 @@
       <c r="H51">
         <v>1.62297E-2</v>
       </c>
-    </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I51">
+        <v>5.4100000000000002E-2</v>
+      </c>
+      <c r="J51">
+        <v>6.9599999999999995E-2</v>
+      </c>
+      <c r="K51">
+        <v>5.5E-2</v>
+      </c>
+    </row>
+    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>1998</v>
       </c>
@@ -1764,8 +2234,17 @@
       <c r="H52">
         <v>1.4268000000000001E-2</v>
       </c>
-    </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I52">
+        <v>4.7100000000000003E-2</v>
+      </c>
+      <c r="J52">
+        <v>6.6400000000000001E-2</v>
+      </c>
+      <c r="K52">
+        <v>4.8099999999999997E-2</v>
+      </c>
+    </row>
+    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>1998</v>
       </c>
@@ -1790,8 +2269,17 @@
       <c r="H53">
         <v>1.6069199999999999E-2</v>
       </c>
-    </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I53">
+        <v>4.5199999999999997E-2</v>
+      </c>
+      <c r="J53">
+        <v>6.83E-2</v>
+      </c>
+      <c r="K53">
+        <v>4.6500000000000007E-2</v>
+      </c>
+    </row>
+    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>1999</v>
       </c>
@@ -1816,8 +2304,17 @@
       <c r="H54">
         <v>1.7284000000000001E-2</v>
       </c>
-    </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I54">
+        <v>4.7800000000000002E-2</v>
+      </c>
+      <c r="J54">
+        <v>6.9800000000000001E-2</v>
+      </c>
+      <c r="K54">
+        <v>5.2300000000000006E-2</v>
+      </c>
+    </row>
+    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>1999</v>
       </c>
@@ -1842,8 +2339,17 @@
       <c r="H55">
         <v>1.9656E-2</v>
       </c>
-    </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I55">
+        <v>5.0999999999999997E-2</v>
+      </c>
+      <c r="J55">
+        <v>7.6300000000000007E-2</v>
+      </c>
+      <c r="K55">
+        <v>5.9000000000000004E-2</v>
+      </c>
+    </row>
+    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>1999</v>
       </c>
@@ -1868,8 +2374,17 @@
       <c r="H56">
         <v>2.6299700000000002E-2</v>
       </c>
-    </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I56">
+        <v>5.2499999999999998E-2</v>
+      </c>
+      <c r="J56">
+        <v>7.7600000000000002E-2</v>
+      </c>
+      <c r="K56">
+        <v>5.9200000000000003E-2</v>
+      </c>
+    </row>
+    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>1999</v>
       </c>
@@ -1894,8 +2409,17 @@
       <c r="H57">
         <v>2.6764000000000003E-2</v>
       </c>
-    </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I57">
+        <v>5.8400000000000001E-2</v>
+      </c>
+      <c r="J57">
+        <v>8.0600000000000005E-2</v>
+      </c>
+      <c r="K57">
+        <v>6.2800000000000009E-2</v>
+      </c>
+    </row>
+    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>2000</v>
       </c>
@@ -1920,8 +2444,17 @@
       <c r="H58">
         <v>3.7621399999999999E-2</v>
       </c>
-    </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I58">
+        <v>6.2199999999999998E-2</v>
+      </c>
+      <c r="J58">
+        <v>8.2300000000000012E-2</v>
+      </c>
+      <c r="K58">
+        <v>6.2600000000000003E-2</v>
+      </c>
+    </row>
+    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>2000</v>
       </c>
@@ -1946,8 +2479,17 @@
       <c r="H59">
         <v>3.7349399999999998E-2</v>
       </c>
-    </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I59">
+        <v>6.1699999999999998E-2</v>
+      </c>
+      <c r="J59">
+        <v>8.2200000000000009E-2</v>
+      </c>
+      <c r="K59">
+        <v>6.0999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>2000</v>
       </c>
@@ -1972,8 +2514,17 @@
       <c r="H60">
         <v>3.4565000000000005E-2</v>
       </c>
-    </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I60">
+        <v>6.13E-2</v>
+      </c>
+      <c r="J60">
+        <v>7.8799999999999995E-2</v>
+      </c>
+      <c r="K60">
+        <v>5.7999999999999996E-2</v>
+      </c>
+    </row>
+    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>2000</v>
       </c>
@@ -1998,8 +2549,17 @@
       <c r="H61">
         <v>3.43602E-2</v>
       </c>
-    </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I61">
+        <v>5.5999999999999994E-2</v>
+      </c>
+      <c r="J61">
+        <v>7.1300000000000002E-2</v>
+      </c>
+      <c r="K61">
+        <v>5.2400000000000002E-2</v>
+      </c>
+    </row>
+    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>2001</v>
       </c>
@@ -2024,8 +2584,17 @@
       <c r="H62">
         <v>2.9824600000000003E-2</v>
       </c>
-    </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I62">
+        <v>4.2999999999999997E-2</v>
+      </c>
+      <c r="J62">
+        <v>6.9100000000000009E-2</v>
+      </c>
+      <c r="K62">
+        <v>4.8899999999999999E-2</v>
+      </c>
+    </row>
+    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>2001</v>
       </c>
@@ -2050,8 +2619,17 @@
       <c r="H63">
         <v>3.1939599999999999E-2</v>
       </c>
-    </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I63">
+        <v>3.5799999999999998E-2</v>
+      </c>
+      <c r="J63">
+        <v>7.110000000000001E-2</v>
+      </c>
+      <c r="K63">
+        <v>5.2800000000000007E-2</v>
+      </c>
+    </row>
+    <row r="64" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>2001</v>
       </c>
@@ -2076,8 +2654,17 @@
       <c r="H64">
         <v>2.5921699999999999E-2</v>
       </c>
-    </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I64">
+        <v>2.8199999999999999E-2</v>
+      </c>
+      <c r="J64">
+        <v>6.7199999999999996E-2</v>
+      </c>
+      <c r="K64">
+        <v>4.7300000000000009E-2</v>
+      </c>
+    </row>
+    <row r="65" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>2001</v>
       </c>
@@ -2102,8 +2689,17 @@
       <c r="H65">
         <v>1.6036700000000001E-2</v>
       </c>
-    </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I65">
+        <v>2.2200000000000001E-2</v>
+      </c>
+      <c r="J65">
+        <v>7.1599999999999997E-2</v>
+      </c>
+      <c r="K65">
+        <v>5.0900000000000001E-2</v>
+      </c>
+    </row>
+    <row r="66" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>2002</v>
       </c>
@@ -2128,8 +2724,17 @@
       <c r="H66">
         <v>1.3628599999999999E-2</v>
       </c>
-    </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I66">
+        <v>2.5700000000000001E-2</v>
+      </c>
+      <c r="J66">
+        <v>7.1800000000000003E-2</v>
+      </c>
+      <c r="K66">
+        <v>5.2800000000000007E-2</v>
+      </c>
+    </row>
+    <row r="67" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>2002</v>
       </c>
@@ -2154,8 +2759,17 @@
       <c r="H67">
         <v>1.0692200000000001E-2</v>
       </c>
-    </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I67">
+        <v>2.2000000000000002E-2</v>
+      </c>
+      <c r="J67">
+        <v>6.5500000000000003E-2</v>
+      </c>
+      <c r="K67">
+        <v>4.9299999999999997E-2</v>
+      </c>
+    </row>
+    <row r="68" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>2002</v>
       </c>
@@ -2180,8 +2794,17 @@
       <c r="H68">
         <v>1.516E-2</v>
       </c>
-    </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I68">
+        <v>1.72E-2</v>
+      </c>
+      <c r="J68">
+        <v>5.9900000000000002E-2</v>
+      </c>
+      <c r="K68">
+        <v>3.8700000000000005E-2</v>
+      </c>
+    </row>
+    <row r="69" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>2002</v>
       </c>
@@ -2206,8 +2829,17 @@
       <c r="H69">
         <v>2.48027E-2</v>
       </c>
-    </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I69">
+        <v>1.4499999999999999E-2</v>
+      </c>
+      <c r="J69">
+        <v>5.9299999999999999E-2</v>
+      </c>
+      <c r="K69">
+        <v>4.0300000000000002E-2</v>
+      </c>
+    </row>
+    <row r="70" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>2003</v>
       </c>
@@ -2232,8 +2864,17 @@
       <c r="H70">
         <v>3.0252100000000001E-2</v>
       </c>
-    </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I70">
+        <v>1.24E-2</v>
+      </c>
+      <c r="J70">
+        <v>5.91E-2</v>
+      </c>
+      <c r="K70">
+        <v>3.8100000000000002E-2</v>
+      </c>
+    </row>
+    <row r="71" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>2003</v>
       </c>
@@ -2258,8 +2899,17 @@
       <c r="H71">
         <v>1.94878E-2</v>
       </c>
-    </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I71">
+        <v>1.01E-2</v>
+      </c>
+      <c r="J71">
+        <v>5.2400000000000002E-2</v>
+      </c>
+      <c r="K71">
+        <v>3.3300000000000003E-2</v>
+      </c>
+    </row>
+    <row r="72" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>2003</v>
       </c>
@@ -2284,8 +2934,17 @@
       <c r="H72">
         <v>2.3783200000000001E-2</v>
       </c>
-    </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I72">
+        <v>1.24E-2</v>
+      </c>
+      <c r="J72">
+        <v>5.9800000000000006E-2</v>
+      </c>
+      <c r="K72">
+        <v>4.2699999999999995E-2</v>
+      </c>
+    </row>
+    <row r="73" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>2003</v>
       </c>
@@ -2310,8 +2969,17 @@
       <c r="H73">
         <v>2.0352000000000002E-2</v>
       </c>
-    </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I73">
+        <v>1.3100000000000001E-2</v>
+      </c>
+      <c r="J73">
+        <v>5.8499999999999996E-2</v>
+      </c>
+      <c r="K73">
+        <v>4.2699999999999995E-2</v>
+      </c>
+    </row>
+    <row r="74" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>2004</v>
       </c>
@@ -2336,8 +3004,17 @@
       <c r="H74">
         <v>1.7400800000000001E-2</v>
       </c>
-    </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I74">
+        <v>1.1899999999999999E-2</v>
+      </c>
+      <c r="J74">
+        <v>5.4000000000000006E-2</v>
+      </c>
+      <c r="K74">
+        <v>3.8300000000000001E-2</v>
+      </c>
+    </row>
+    <row r="75" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>2004</v>
       </c>
@@ -2362,8 +3039,17 @@
       <c r="H75">
         <v>3.1676700000000002E-2</v>
       </c>
-    </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I75">
+        <v>2.12E-2</v>
+      </c>
+      <c r="J75">
+        <v>6.25E-2</v>
+      </c>
+      <c r="K75">
+        <v>4.7300000000000009E-2</v>
+      </c>
+    </row>
+    <row r="76" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>2004</v>
       </c>
@@ -2388,8 +3074,17 @@
       <c r="H76">
         <v>2.53917E-2</v>
       </c>
-    </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I76">
+        <v>2.12E-2</v>
+      </c>
+      <c r="J76">
+        <v>5.7200000000000001E-2</v>
+      </c>
+      <c r="K76">
+        <v>4.1299999999999996E-2</v>
+      </c>
+    </row>
+    <row r="77" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A77">
         <v>2004</v>
       </c>
@@ -2414,8 +3109,17 @@
       <c r="H77">
         <v>3.34232E-2</v>
       </c>
-    </row>
-    <row r="78" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I77">
+        <v>2.6700000000000002E-2</v>
+      </c>
+      <c r="J77">
+        <v>5.8099999999999999E-2</v>
+      </c>
+      <c r="K77">
+        <v>4.2300000000000004E-2</v>
+      </c>
+    </row>
+    <row r="78" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A78">
         <v>2005</v>
       </c>
@@ -2440,8 +3144,17 @@
       <c r="H78">
         <v>3.2068400000000004E-2</v>
       </c>
-    </row>
-    <row r="79" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I78">
+        <v>3.3000000000000002E-2</v>
+      </c>
+      <c r="J78">
+        <v>6.0400000000000002E-2</v>
+      </c>
+      <c r="K78">
+        <v>4.4999999999999998E-2</v>
+      </c>
+    </row>
+    <row r="79" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A79">
         <v>2005</v>
       </c>
@@ -2466,8 +3179,17 @@
       <c r="H79">
         <v>2.54103E-2</v>
       </c>
-    </row>
-    <row r="80" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I79">
+        <v>3.3599999999999998E-2</v>
+      </c>
+      <c r="J79">
+        <v>5.5300000000000002E-2</v>
+      </c>
+      <c r="K79">
+        <v>0.04</v>
+      </c>
+    </row>
+    <row r="80" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A80">
         <v>2005</v>
       </c>
@@ -2492,8 +3214,17 @@
       <c r="H80">
         <v>4.7418300000000004E-2</v>
       </c>
-    </row>
-    <row r="81" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I80">
+        <v>3.85E-2</v>
+      </c>
+      <c r="J80">
+        <v>5.91E-2</v>
+      </c>
+      <c r="K80">
+        <v>4.2000000000000003E-2</v>
+      </c>
+    </row>
+    <row r="81" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A81">
         <v>2005</v>
       </c>
@@ -2518,8 +3249,17 @@
       <c r="H81">
         <v>3.3385499999999999E-2</v>
       </c>
-    </row>
-    <row r="82" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I81">
+        <v>4.3499999999999997E-2</v>
+      </c>
+      <c r="J81">
+        <v>6.2199999999999998E-2</v>
+      </c>
+      <c r="K81">
+        <v>4.4699999999999997E-2</v>
+      </c>
+    </row>
+    <row r="82" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A82">
         <v>2006</v>
       </c>
@@ -2544,8 +3284,17 @@
       <c r="H82">
         <v>3.41792E-2</v>
       </c>
-    </row>
-    <row r="83" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I82">
+        <v>4.7699999999999999E-2</v>
+      </c>
+      <c r="J82">
+        <v>6.3500000000000001E-2</v>
+      </c>
+      <c r="K82">
+        <v>4.7199999999999999E-2</v>
+      </c>
+    </row>
+    <row r="83" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A83">
         <v>2006</v>
       </c>
@@ -2570,8 +3319,17 @@
       <c r="H83">
         <v>4.1817200000000006E-2</v>
       </c>
-    </row>
-    <row r="84" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I83">
+        <v>5.16E-2</v>
+      </c>
+      <c r="J83">
+        <v>6.7799999999999999E-2</v>
+      </c>
+      <c r="K83">
+        <v>5.1100000000000007E-2</v>
+      </c>
+    </row>
+    <row r="84" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A84">
         <v>2006</v>
       </c>
@@ -2596,8 +3354,17 @@
       <c r="H84">
         <v>2.0120700000000002E-2</v>
       </c>
-    </row>
-    <row r="85" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I84">
+        <v>4.9700000000000001E-2</v>
+      </c>
+      <c r="J84">
+        <v>6.3100000000000003E-2</v>
+      </c>
+      <c r="K84">
+        <v>4.7199999999999999E-2</v>
+      </c>
+    </row>
+    <row r="85" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A85">
         <v>2006</v>
       </c>
@@ -2622,8 +3389,17 @@
       <c r="H85">
         <v>2.52398E-2</v>
       </c>
-    </row>
-    <row r="86" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I85">
+        <v>4.9400000000000006E-2</v>
+      </c>
+      <c r="J85">
+        <v>6.1800000000000001E-2</v>
+      </c>
+      <c r="K85">
+        <v>4.5599999999999995E-2</v>
+      </c>
+    </row>
+    <row r="86" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A86">
         <v>2007</v>
       </c>
@@ -2648,8 +3424,17 @@
       <c r="H86">
         <v>2.7982E-2</v>
       </c>
-    </row>
-    <row r="87" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I86">
+        <v>4.9200000000000001E-2</v>
+      </c>
+      <c r="J86">
+        <v>6.1600000000000002E-2</v>
+      </c>
+      <c r="K86">
+        <v>4.5599999999999995E-2</v>
+      </c>
+    </row>
+    <row r="87" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A87">
         <v>2007</v>
       </c>
@@ -2674,8 +3459,17 @@
       <c r="H87">
         <v>2.6927699999999999E-2</v>
       </c>
-    </row>
-    <row r="88" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I87">
+        <v>4.9599999999999998E-2</v>
+      </c>
+      <c r="J87">
+        <v>6.6699999999999995E-2</v>
+      </c>
+      <c r="K87">
+        <v>5.0999999999999997E-2</v>
+      </c>
+    </row>
+    <row r="88" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A88">
         <v>2007</v>
       </c>
@@ -2700,8 +3494,17 @@
       <c r="H88">
         <v>2.83383E-2</v>
       </c>
-    </row>
-    <row r="89" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I88">
+        <v>4.1399999999999999E-2</v>
+      </c>
+      <c r="J88">
+        <v>6.4200000000000007E-2</v>
+      </c>
+      <c r="K88">
+        <v>4.5199999999999997E-2</v>
+      </c>
+    </row>
+    <row r="89" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A89">
         <v>2007</v>
       </c>
@@ -2726,8 +3529,17 @@
       <c r="H89">
         <v>4.1088100000000002E-2</v>
       </c>
-    </row>
-    <row r="90" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I89">
+        <v>3.2599999999999997E-2</v>
+      </c>
+      <c r="J89">
+        <v>6.1699999999999998E-2</v>
+      </c>
+      <c r="K89">
+        <v>4.0999999999999995E-2</v>
+      </c>
+    </row>
+    <row r="90" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A90">
         <v>2008</v>
       </c>
@@ -2752,8 +3564,17 @@
       <c r="H90">
         <v>3.9749E-2</v>
       </c>
-    </row>
-    <row r="91" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I90">
+        <v>1.54E-2</v>
+      </c>
+      <c r="J90">
+        <v>5.8499999999999996E-2</v>
+      </c>
+      <c r="K90">
+        <v>3.5099999999999999E-2</v>
+      </c>
+    </row>
+    <row r="91" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A91">
         <v>2008</v>
       </c>
@@ -2778,8 +3599,17 @@
       <c r="H91">
         <v>4.9359700000000006E-2</v>
       </c>
-    </row>
-    <row r="92" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I91">
+        <v>2.4199999999999999E-2</v>
+      </c>
+      <c r="J91">
+        <v>6.4500000000000002E-2</v>
+      </c>
+      <c r="K91">
+        <v>4.0999999999999995E-2</v>
+      </c>
+    </row>
+    <row r="92" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A92">
         <v>2008</v>
       </c>
@@ -2804,8 +3634,17 @@
       <c r="H92">
         <v>4.9533199999999999E-2</v>
       </c>
-    </row>
-    <row r="93" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I92">
+        <v>1.9099999999999999E-2</v>
+      </c>
+      <c r="J92">
+        <v>6.0900000000000003E-2</v>
+      </c>
+      <c r="K92">
+        <v>3.6900000000000002E-2</v>
+      </c>
+    </row>
+    <row r="93" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A93">
         <v>2008</v>
       </c>
@@ -2830,8 +3669,17 @@
       <c r="H93">
         <v>-2.2230000000000001E-4</v>
       </c>
-    </row>
-    <row r="94" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I93">
+        <v>4.8999999999999998E-3</v>
+      </c>
+      <c r="J93">
+        <v>5.0999999999999997E-2</v>
+      </c>
+      <c r="K93">
+        <v>2.4199999999999999E-2</v>
+      </c>
+    </row>
+    <row r="94" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A94">
         <v>2009</v>
       </c>
@@ -2856,8 +3704,17 @@
       <c r="H94">
         <v>-4.4647999999999997E-3</v>
       </c>
-    </row>
-    <row r="95" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I94">
+        <v>6.4000000000000003E-3</v>
+      </c>
+      <c r="J94">
+        <v>4.8499999999999995E-2</v>
+      </c>
+      <c r="K94">
+        <v>2.8199999999999999E-2</v>
+      </c>
+    </row>
+    <row r="95" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A95">
         <v>2009</v>
       </c>
@@ -2882,8 +3739,17 @@
       <c r="H95">
         <v>-1.2291700000000001E-2</v>
       </c>
-    </row>
-    <row r="96" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I95">
+        <v>5.1000000000000004E-3</v>
+      </c>
+      <c r="J95">
+        <v>5.4199999999999998E-2</v>
+      </c>
+      <c r="K95">
+        <v>3.7200000000000004E-2</v>
+      </c>
+    </row>
+    <row r="96" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A96">
         <v>2009</v>
       </c>
@@ -2908,8 +3774,17 @@
       <c r="H96">
         <v>-1.3779399999999999E-2</v>
       </c>
-    </row>
-    <row r="97" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I96">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="J96">
+        <v>5.04E-2</v>
+      </c>
+      <c r="K96">
+        <v>3.4000000000000002E-2</v>
+      </c>
+    </row>
+    <row r="97" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A97">
         <v>2009</v>
       </c>
@@ -2934,8 +3809,17 @@
       <c r="H97">
         <v>2.8141200000000002E-2</v>
       </c>
-    </row>
-    <row r="98" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I97">
+        <v>3.7000000000000002E-3</v>
+      </c>
+      <c r="J97">
+        <v>5.1400000000000001E-2</v>
+      </c>
+      <c r="K97">
+        <v>3.5900000000000001E-2</v>
+      </c>
+    </row>
+    <row r="98" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A98">
         <v>2010</v>
       </c>
@@ -2960,8 +3844,17 @@
       <c r="H98">
         <v>2.2861699999999999E-2</v>
       </c>
-    </row>
-    <row r="99" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I98">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="J98">
+        <v>4.99E-2</v>
+      </c>
+      <c r="K98">
+        <v>3.73E-2</v>
+      </c>
+    </row>
+    <row r="99" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A99">
         <v>2010</v>
       </c>
@@ -2986,8 +3879,17 @@
       <c r="H99">
         <v>1.1215599999999999E-2</v>
       </c>
-    </row>
-    <row r="100" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I99">
+        <v>3.2000000000000002E-3</v>
+      </c>
+      <c r="J99">
+        <v>4.6900000000000004E-2</v>
+      </c>
+      <c r="K99">
+        <v>3.2000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="100" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A100">
         <v>2010</v>
       </c>
@@ -3012,8 +3914,17 @@
       <c r="H100">
         <v>1.11831E-2</v>
       </c>
-    </row>
-    <row r="101" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I100">
+        <v>2.6000000000000003E-3</v>
+      </c>
+      <c r="J100">
+        <v>4.3200000000000002E-2</v>
+      </c>
+      <c r="K100">
+        <v>2.6499999999999999E-2</v>
+      </c>
+    </row>
+    <row r="101" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A101">
         <v>2010</v>
       </c>
@@ -3038,8 +3949,17 @@
       <c r="H101">
         <v>1.4377899999999999E-2</v>
       </c>
-    </row>
-    <row r="102" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I101">
+        <v>2.8999999999999998E-3</v>
+      </c>
+      <c r="J101">
+        <v>4.8600000000000004E-2</v>
+      </c>
+      <c r="K101">
+        <v>3.2899999999999999E-2</v>
+      </c>
+    </row>
+    <row r="102" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A102">
         <v>2011</v>
       </c>
@@ -3064,8 +3984,17 @@
       <c r="H102">
         <v>2.6192400000000001E-2</v>
       </c>
-    </row>
-    <row r="103" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I102">
+        <v>2.6000000000000003E-3</v>
+      </c>
+      <c r="J102">
+        <v>4.8600000000000004E-2</v>
+      </c>
+      <c r="K102">
+        <v>3.4100000000000005E-2</v>
+      </c>
+    </row>
+    <row r="103" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A103">
         <v>2011</v>
       </c>
@@ -3090,8 +4019,17 @@
       <c r="H103">
         <v>3.5023200000000004E-2</v>
       </c>
-    </row>
-    <row r="104" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I103">
+        <v>1.8E-3</v>
+      </c>
+      <c r="J103">
+        <v>4.5100000000000001E-2</v>
+      </c>
+      <c r="K103">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="104" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A104">
         <v>2011</v>
       </c>
@@ -3116,8 +4054,17 @@
       <c r="H104">
         <v>3.8126199999999999E-2</v>
       </c>
-    </row>
-    <row r="105" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I104">
+        <v>1E-3</v>
+      </c>
+      <c r="J104">
+        <v>4.0099999999999997E-2</v>
+      </c>
+      <c r="K104">
+        <v>1.9800000000000002E-2</v>
+      </c>
+    </row>
+    <row r="105" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A105">
         <v>2011</v>
       </c>
@@ -3142,8 +4089,17 @@
       <c r="H105">
         <v>3.0620700000000001E-2</v>
       </c>
-    </row>
-    <row r="106" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I105">
+        <v>1.1999999999999999E-3</v>
+      </c>
+      <c r="J105">
+        <v>3.95E-2</v>
+      </c>
+      <c r="K105">
+        <v>1.9800000000000002E-2</v>
+      </c>
+    </row>
+    <row r="106" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A106">
         <v>2012</v>
       </c>
@@ -3168,8 +4124,17 @@
       <c r="H106">
         <v>2.62188E-2</v>
       </c>
-    </row>
-    <row r="107" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I106">
+        <v>1.9E-3</v>
+      </c>
+      <c r="J106">
+        <v>3.9900000000000005E-2</v>
+      </c>
+      <c r="K106">
+        <v>2.1700000000000001E-2</v>
+      </c>
+    </row>
+    <row r="107" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A107">
         <v>2012</v>
       </c>
@@ -3194,8 +4159,17 @@
       <c r="H107">
         <v>1.64586E-2</v>
       </c>
-    </row>
-    <row r="108" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I107">
+        <v>1.9E-3</v>
+      </c>
+      <c r="J107">
+        <v>3.6600000000000001E-2</v>
+      </c>
+      <c r="K107">
+        <v>1.6200000000000003E-2</v>
+      </c>
+    </row>
+    <row r="108" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A108">
         <v>2012</v>
       </c>
@@ -3220,8 +4194,17 @@
       <c r="H108">
         <v>1.9373600000000001E-2</v>
       </c>
-    </row>
-    <row r="109" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I108">
+        <v>1.8E-3</v>
+      </c>
+      <c r="J108">
+        <v>3.4000000000000002E-2</v>
+      </c>
+      <c r="K108">
+        <v>1.72E-2</v>
+      </c>
+    </row>
+    <row r="109" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A109">
         <v>2012</v>
       </c>
@@ -3246,8 +4229,17 @@
       <c r="H109">
         <v>1.7819499999999999E-2</v>
       </c>
-    </row>
-    <row r="110" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I109">
+        <v>1.6000000000000001E-3</v>
+      </c>
+      <c r="J109">
+        <v>3.3500000000000002E-2</v>
+      </c>
+      <c r="K109">
+        <v>1.72E-2</v>
+      </c>
+    </row>
+    <row r="110" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A110">
         <v>2013</v>
       </c>
@@ -3272,8 +4264,17 @@
       <c r="H110">
         <v>1.4937000000000001E-2</v>
       </c>
-    </row>
-    <row r="111" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I110">
+        <v>1.5E-3</v>
+      </c>
+      <c r="J110">
+        <v>3.5700000000000003E-2</v>
+      </c>
+      <c r="K110">
+        <v>1.9599999999999999E-2</v>
+      </c>
+    </row>
+    <row r="111" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A111">
         <v>2013</v>
       </c>
@@ -3298,8 +4299,17 @@
       <c r="H111">
         <v>1.6852900000000001E-2</v>
       </c>
-    </row>
-    <row r="112" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I111">
+        <v>1.4000000000000002E-3</v>
+      </c>
+      <c r="J111">
+        <v>4.4600000000000001E-2</v>
+      </c>
+      <c r="K111">
+        <v>2.3E-2</v>
+      </c>
+    </row>
+    <row r="112" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A112">
         <v>2013</v>
       </c>
@@ -3324,8 +4334,17 @@
       <c r="H112">
         <v>1.1494200000000001E-2</v>
       </c>
-    </row>
-    <row r="113" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I112">
+        <v>1.1999999999999999E-3</v>
+      </c>
+      <c r="J112">
+        <v>4.3200000000000002E-2</v>
+      </c>
+      <c r="K112">
+        <v>2.81E-2</v>
+      </c>
+    </row>
+    <row r="113" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A113">
         <v>2013</v>
       </c>
@@ -3350,8 +4369,17 @@
       <c r="H113">
         <v>1.5458000000000001E-2</v>
       </c>
-    </row>
-    <row r="114" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I113">
+        <v>1.3000000000000002E-3</v>
+      </c>
+      <c r="J113">
+        <v>4.4800000000000006E-2</v>
+      </c>
+      <c r="K113">
+        <v>2.8999999999999998E-2</v>
+      </c>
+    </row>
+    <row r="114" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A114">
         <v>2014</v>
       </c>
@@ -3375,6 +4403,15 @@
       </c>
       <c r="H114">
         <v>1.54275E-2</v>
+      </c>
+      <c r="I114">
+        <v>1.3000000000000002E-3</v>
+      </c>
+      <c r="J114">
+        <v>4.4000000000000004E-2</v>
+      </c>
+      <c r="K114">
+        <v>2.7200000000000002E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>